<commit_message>
added data from new studies
</commit_message>
<xml_diff>
--- a/data/MSdata.xlsx
+++ b/data/MSdata.xlsx
@@ -17,11 +17,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="439">
   <si>
     <t>id</t>
   </si>
@@ -1251,6 +1252,93 @@
   </si>
   <si>
     <t>Brisbane</t>
+  </si>
+  <si>
+    <t>Birds and the urban environment: the value of green walls</t>
+  </si>
+  <si>
+    <t>Chiquet, C., Dover, J.W., &amp; Mitchell, P.</t>
+  </si>
+  <si>
+    <t>bird abundance</t>
+  </si>
+  <si>
+    <t>Newcastle-under-Lyme</t>
+  </si>
+  <si>
+    <t>green walls</t>
+  </si>
+  <si>
+    <t>Ground-Nesting Birds on Green Roofs in Switzerland: Preliminary Observations</t>
+  </si>
+  <si>
+    <t>Baumann, N.</t>
+  </si>
+  <si>
+    <t>Green Roofs – Urban Habitats for Ground-Nesting Birds and Plants</t>
+  </si>
+  <si>
+    <t>Baumann, N. &amp; Kasten, F.</t>
+  </si>
+  <si>
+    <t>Urban Biodiversity and Design</t>
+  </si>
+  <si>
+    <t>bird survival</t>
+  </si>
+  <si>
+    <t>Insect and avian fauna presence on the Ford assembly plant ecoroof</t>
+  </si>
+  <si>
+    <t>Coffman, R. &amp; Davis, G.</t>
+  </si>
+  <si>
+    <t>Third annual greening rooftops for sustainable communities conference, awards and trade show</t>
+  </si>
+  <si>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>Can green roofs provide habitat for urban bees (Hymenoptera: Apidae)?</t>
+  </si>
+  <si>
+    <t>Colla, S., Willis, &amp; Packer, L.</t>
+  </si>
+  <si>
+    <t>Cities and the Environment</t>
+  </si>
+  <si>
+    <t>An assessment of pollen limitation on Chicago green roofs</t>
+  </si>
+  <si>
+    <t>Ksiazek, K., Fant, J., &amp; Skogena, K.</t>
+  </si>
+  <si>
+    <t>Landscape and Urban Planning</t>
+  </si>
+  <si>
+    <t>A comparison of bee communities of Chicago green roofs, parks and prairies</t>
+  </si>
+  <si>
+    <t>Tonietto, R., Fant, J., Ascher, K., Ellis, D., &amp; Larkin, D.</t>
+  </si>
+  <si>
+    <t>Madre, F., Vergnes, A., Machon, N.,  &amp; Clergeau, P</t>
+  </si>
+  <si>
+    <t>A comparison of 3 types of green roof as habitats for arthropods</t>
+  </si>
+  <si>
+    <t>Ecological Engineering</t>
+  </si>
+  <si>
+    <t>Building biodiversity: Vegetated façades as habitats for spider and beetle assemblages</t>
+  </si>
+  <si>
+    <t>Madre, F., Clergeau, P., Machon, N.,  &amp; Vergnes, A.</t>
+  </si>
+  <si>
+    <t>Global Ecology and Conservation</t>
   </si>
 </sst>
 </file>
@@ -1286,11 +1374,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1595,10 +1680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y102"/>
+  <dimension ref="A1:XFD111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M111" sqref="M111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4246,7 +4331,7 @@
       <c r="A59">
         <v>949</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>405</v>
       </c>
       <c r="C59" t="s">
@@ -5848,7 +5933,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1265</v>
       </c>
@@ -5895,7 +5980,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1267</v>
       </c>
@@ -5924,7 +6009,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1269</v>
       </c>
@@ -5968,7 +6053,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1273</v>
       </c>
@@ -5997,7 +6082,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1274</v>
       </c>
@@ -6041,7 +6126,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1285</v>
       </c>
@@ -6088,8 +6173,345 @@
         <v>5</v>
       </c>
     </row>
+    <row r="103" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1286</v>
+      </c>
+      <c r="B103" t="s">
+        <v>410</v>
+      </c>
+      <c r="C103" t="s">
+        <v>411</v>
+      </c>
+      <c r="D103" t="s">
+        <v>270</v>
+      </c>
+      <c r="E103">
+        <v>2013</v>
+      </c>
+      <c r="H103">
+        <v>53.010899999999999</v>
+      </c>
+      <c r="I103">
+        <v>-2.2277999999999998</v>
+      </c>
+      <c r="J103">
+        <v>124</v>
+      </c>
+      <c r="K103" t="s">
+        <v>413</v>
+      </c>
+      <c r="L103" t="s">
+        <v>141</v>
+      </c>
+      <c r="M103">
+        <v>0.12826399999999999</v>
+      </c>
+      <c r="N103">
+        <v>6.0800000000000003E-3</v>
+      </c>
+      <c r="O103" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1287</v>
+      </c>
+      <c r="B104" t="s">
+        <v>415</v>
+      </c>
+      <c r="C104" t="s">
+        <v>416</v>
+      </c>
+      <c r="D104" t="s">
+        <v>289</v>
+      </c>
+      <c r="E104">
+        <v>2006</v>
+      </c>
+      <c r="L104" t="s">
+        <v>176</v>
+      </c>
+      <c r="O104" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="105" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1288</v>
+      </c>
+      <c r="B105" t="s">
+        <v>417</v>
+      </c>
+      <c r="C105" t="s">
+        <v>418</v>
+      </c>
+      <c r="D105" t="s">
+        <v>419</v>
+      </c>
+      <c r="E105">
+        <v>2010</v>
+      </c>
+      <c r="F105" t="s">
+        <v>396</v>
+      </c>
+      <c r="L105" t="s">
+        <v>176</v>
+      </c>
+      <c r="O105" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="106" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>1289</v>
+      </c>
+      <c r="B106" t="s">
+        <v>421</v>
+      </c>
+      <c r="C106" t="s">
+        <v>422</v>
+      </c>
+      <c r="D106" t="s">
+        <v>423</v>
+      </c>
+      <c r="E106">
+        <v>2005</v>
+      </c>
+      <c r="F106" t="s">
+        <v>396</v>
+      </c>
+      <c r="H106">
+        <v>43.256667</v>
+      </c>
+      <c r="I106">
+        <v>-79.869167000000004</v>
+      </c>
+      <c r="J106">
+        <v>96</v>
+      </c>
+      <c r="K106" t="s">
+        <v>424</v>
+      </c>
+      <c r="L106" t="s">
+        <v>53</v>
+      </c>
+      <c r="M106">
+        <v>0.53691699999999998</v>
+      </c>
+      <c r="N106">
+        <v>4.7199999999999998E-4</v>
+      </c>
+      <c r="O106" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="107" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1290</v>
+      </c>
+      <c r="B107" t="s">
+        <v>425</v>
+      </c>
+      <c r="C107" t="s">
+        <v>426</v>
+      </c>
+      <c r="D107" t="s">
+        <v>427</v>
+      </c>
+      <c r="E107">
+        <v>2009</v>
+      </c>
+      <c r="F107" t="s">
+        <v>26</v>
+      </c>
+      <c r="H107">
+        <v>43.7</v>
+      </c>
+      <c r="I107">
+        <v>-79.400000000000006</v>
+      </c>
+      <c r="J107">
+        <v>76</v>
+      </c>
+      <c r="K107" t="s">
+        <v>52</v>
+      </c>
+      <c r="L107" t="s">
+        <v>53</v>
+      </c>
+      <c r="M107">
+        <v>5.1327939999999996</v>
+      </c>
+      <c r="N107">
+        <v>2.931E-3</v>
+      </c>
+      <c r="O107" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="108" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>1291</v>
+      </c>
+      <c r="B108" t="s">
+        <v>428</v>
+      </c>
+      <c r="C108" t="s">
+        <v>429</v>
+      </c>
+      <c r="D108" t="s">
+        <v>430</v>
+      </c>
+      <c r="E108">
+        <v>2012</v>
+      </c>
+      <c r="H108">
+        <v>41.836944000000003</v>
+      </c>
+      <c r="I108">
+        <v>-87.684721999999994</v>
+      </c>
+      <c r="K108" t="s">
+        <v>261</v>
+      </c>
+      <c r="L108" t="s">
+        <v>37</v>
+      </c>
+      <c r="M108">
+        <v>2.6949999999999998</v>
+      </c>
+      <c r="N108">
+        <v>1.157E-2</v>
+      </c>
+      <c r="O108" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="109" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1292</v>
+      </c>
+      <c r="B109" t="s">
+        <v>431</v>
+      </c>
+      <c r="C109" t="s">
+        <v>432</v>
+      </c>
+      <c r="D109" t="s">
+        <v>430</v>
+      </c>
+      <c r="E109">
+        <v>2011</v>
+      </c>
+      <c r="H109">
+        <v>41.836944000000003</v>
+      </c>
+      <c r="I109">
+        <v>-87.684721999999994</v>
+      </c>
+      <c r="K109" t="s">
+        <v>261</v>
+      </c>
+      <c r="L109" t="s">
+        <v>37</v>
+      </c>
+      <c r="M109">
+        <v>2.6949999999999998</v>
+      </c>
+      <c r="N109">
+        <v>1.157E-2</v>
+      </c>
+      <c r="O109" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="110" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1293</v>
+      </c>
+      <c r="B110" t="s">
+        <v>434</v>
+      </c>
+      <c r="C110" t="s">
+        <v>433</v>
+      </c>
+      <c r="D110" t="s">
+        <v>435</v>
+      </c>
+      <c r="E110">
+        <v>2013</v>
+      </c>
+      <c r="F110" t="s">
+        <v>396</v>
+      </c>
+      <c r="L110" t="s">
+        <v>27</v>
+      </c>
+      <c r="O110" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="111" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1294</v>
+      </c>
+      <c r="B111" t="s">
+        <v>436</v>
+      </c>
+      <c r="C111" t="s">
+        <v>437</v>
+      </c>
+      <c r="D111" t="s">
+        <v>438</v>
+      </c>
+      <c r="E111">
+        <v>2015</v>
+      </c>
+      <c r="F111" t="s">
+        <v>26</v>
+      </c>
+      <c r="L111" t="s">
+        <v>27</v>
+      </c>
+      <c r="O111" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>267</v>
+      </c>
+      <c r="XFD111">
+        <v>2013</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added 5 more datasets and contacted additional authors
</commit_message>
<xml_diff>
--- a/data/MSdata.xlsx
+++ b/data/MSdata.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PhD - 10th Year\GreenInfrastructureMeta\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="660" windowWidth="28275" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="471">
   <si>
     <t>id</t>
   </si>
@@ -1437,8 +1432,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1529,7 +1524,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1561,10 +1556,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1596,7 +1590,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1772,19 +1765,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1861,7 +1854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="A2">
         <v>39</v>
       </c>
@@ -1896,7 +1889,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="A3">
         <v>69</v>
       </c>
@@ -1949,7 +1942,7 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="A4">
         <v>95</v>
       </c>
@@ -1993,7 +1986,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="A5">
         <v>104</v>
       </c>
@@ -2040,7 +2033,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="A6">
         <v>150</v>
       </c>
@@ -2096,7 +2089,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7">
         <v>154</v>
       </c>
@@ -2143,7 +2136,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="A8">
         <v>161</v>
       </c>
@@ -2193,7 +2186,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="A9">
         <v>189</v>
       </c>
@@ -2243,7 +2236,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25">
       <c r="A10">
         <v>247</v>
       </c>
@@ -2287,7 +2280,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25">
       <c r="A11">
         <v>251</v>
       </c>
@@ -2334,7 +2327,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12">
         <v>253</v>
       </c>
@@ -2384,7 +2377,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="A13">
         <v>310</v>
       </c>
@@ -2431,7 +2424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="A14">
         <v>315</v>
       </c>
@@ -2463,7 +2456,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="A15">
         <v>319</v>
       </c>
@@ -2516,7 +2509,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="A16">
         <v>328</v>
       </c>
@@ -2563,7 +2556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17">
         <v>335</v>
       </c>
@@ -2610,7 +2603,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18">
         <v>356</v>
       </c>
@@ -2660,7 +2653,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19">
         <v>364</v>
       </c>
@@ -2707,7 +2700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20">
         <v>397</v>
       </c>
@@ -2739,7 +2732,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21">
         <v>400</v>
       </c>
@@ -2789,7 +2782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22">
         <v>408</v>
       </c>
@@ -2821,7 +2814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23">
         <v>415</v>
       </c>
@@ -2871,7 +2864,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24">
         <v>429</v>
       </c>
@@ -2918,7 +2911,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25">
         <v>431</v>
       </c>
@@ -2950,7 +2943,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26">
         <v>434</v>
       </c>
@@ -2997,7 +2990,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27">
         <v>454</v>
       </c>
@@ -3044,7 +3037,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28">
         <v>463</v>
       </c>
@@ -3091,7 +3084,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="A29">
         <v>464</v>
       </c>
@@ -3138,7 +3131,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
       <c r="A30">
         <v>465</v>
       </c>
@@ -3164,7 +3157,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22">
       <c r="A31">
         <v>466</v>
       </c>
@@ -3217,7 +3210,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="A32">
         <v>491</v>
       </c>
@@ -3261,7 +3254,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22">
       <c r="A33">
         <v>499</v>
       </c>
@@ -3308,7 +3301,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22">
       <c r="A34">
         <v>511</v>
       </c>
@@ -3340,7 +3333,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22">
       <c r="A35">
         <v>514</v>
       </c>
@@ -3393,7 +3386,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22">
       <c r="A36">
         <v>536</v>
       </c>
@@ -3449,7 +3442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22">
       <c r="A37">
         <v>546</v>
       </c>
@@ -3493,7 +3486,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22">
       <c r="A38">
         <v>563</v>
       </c>
@@ -3540,7 +3533,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22">
       <c r="A39">
         <v>593</v>
       </c>
@@ -3581,7 +3574,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22">
       <c r="A40">
         <v>621</v>
       </c>
@@ -3622,7 +3615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22">
       <c r="A41">
         <v>640</v>
       </c>
@@ -3669,7 +3662,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22">
       <c r="A42">
         <v>641</v>
       </c>
@@ -3719,7 +3712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22">
       <c r="A43">
         <v>659</v>
       </c>
@@ -3769,7 +3762,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22">
       <c r="A44">
         <v>670</v>
       </c>
@@ -3798,7 +3791,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22">
       <c r="A45">
         <v>679</v>
       </c>
@@ -3848,7 +3841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22">
       <c r="A46">
         <v>697</v>
       </c>
@@ -3895,7 +3888,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22">
       <c r="A47">
         <v>728</v>
       </c>
@@ -3924,7 +3917,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22">
       <c r="A48">
         <v>760</v>
       </c>
@@ -3971,7 +3964,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24">
       <c r="A49">
         <v>777</v>
       </c>
@@ -4018,7 +4011,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24">
       <c r="A50">
         <v>787</v>
       </c>
@@ -4065,7 +4058,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24">
       <c r="A51">
         <v>800</v>
       </c>
@@ -4094,7 +4087,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24">
       <c r="A52">
         <v>877</v>
       </c>
@@ -4135,7 +4128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24">
       <c r="A53">
         <v>879</v>
       </c>
@@ -4185,7 +4178,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24">
       <c r="A54">
         <v>881</v>
       </c>
@@ -4235,7 +4228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24">
       <c r="A55">
         <v>895</v>
       </c>
@@ -4285,7 +4278,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24">
       <c r="A56">
         <v>899</v>
       </c>
@@ -4335,7 +4328,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24">
       <c r="A57">
         <v>912</v>
       </c>
@@ -4376,7 +4369,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24">
       <c r="A58">
         <v>926</v>
       </c>
@@ -4423,7 +4416,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24">
       <c r="A59">
         <v>949</v>
       </c>
@@ -4461,7 +4454,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24">
       <c r="A60">
         <v>976</v>
       </c>
@@ -4511,7 +4504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24">
       <c r="A61">
         <v>1023</v>
       </c>
@@ -4555,7 +4548,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24">
       <c r="A62">
         <v>1046</v>
       </c>
@@ -4596,7 +4589,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24">
       <c r="A63">
         <v>1047</v>
       </c>
@@ -4637,7 +4630,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24">
       <c r="A64">
         <v>1049</v>
       </c>
@@ -4687,7 +4680,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22">
       <c r="A65">
         <v>1050</v>
       </c>
@@ -4740,7 +4733,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22">
       <c r="A66">
         <v>1051</v>
       </c>
@@ -4796,7 +4789,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22">
       <c r="A67">
         <v>1052</v>
       </c>
@@ -4843,7 +4836,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22">
       <c r="A68">
         <v>1055</v>
       </c>
@@ -4893,7 +4886,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22">
       <c r="A69">
         <v>1056</v>
       </c>
@@ -4940,7 +4933,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22">
       <c r="A70">
         <v>1059</v>
       </c>
@@ -4972,7 +4965,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22">
       <c r="A71">
         <v>1062</v>
       </c>
@@ -4988,6 +4981,9 @@
       <c r="E71">
         <v>2011</v>
       </c>
+      <c r="F71" t="s">
+        <v>396</v>
+      </c>
       <c r="H71">
         <v>52.483055999999998</v>
       </c>
@@ -5019,7 +5015,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22">
       <c r="A72">
         <v>1063</v>
       </c>
@@ -5035,6 +5031,9 @@
       <c r="E72">
         <v>2009</v>
       </c>
+      <c r="F72" t="s">
+        <v>396</v>
+      </c>
       <c r="H72">
         <v>59.329444000000002</v>
       </c>
@@ -5066,7 +5065,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22">
       <c r="A73">
         <v>1067</v>
       </c>
@@ -5082,6 +5081,9 @@
       <c r="E73">
         <v>1999</v>
       </c>
+      <c r="F73" t="s">
+        <v>400</v>
+      </c>
       <c r="H73">
         <v>52.204999999999998</v>
       </c>
@@ -5110,7 +5112,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22">
       <c r="A74">
         <v>1069</v>
       </c>
@@ -5126,6 +5128,9 @@
       <c r="E74">
         <v>2012</v>
       </c>
+      <c r="F74" t="s">
+        <v>396</v>
+      </c>
       <c r="H74">
         <v>52.4</v>
       </c>
@@ -5154,7 +5159,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22">
       <c r="A75">
         <v>1070</v>
       </c>
@@ -5170,6 +5175,9 @@
       <c r="E75">
         <v>2008</v>
       </c>
+      <c r="F75" t="s">
+        <v>400</v>
+      </c>
       <c r="H75">
         <v>40.712777799999998</v>
       </c>
@@ -5198,7 +5206,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22">
       <c r="A76">
         <v>1076</v>
       </c>
@@ -5214,6 +5222,9 @@
       <c r="E76">
         <v>2014</v>
       </c>
+      <c r="F76" t="s">
+        <v>26</v>
+      </c>
       <c r="H76">
         <v>48.856699999999996</v>
       </c>
@@ -5239,7 +5250,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22">
       <c r="A77">
         <v>1093</v>
       </c>
@@ -5255,6 +5266,9 @@
       <c r="E77">
         <v>2013</v>
       </c>
+      <c r="F77" t="s">
+        <v>396</v>
+      </c>
       <c r="H77">
         <v>40.712777799999998</v>
       </c>
@@ -5286,7 +5300,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22">
       <c r="A78">
         <v>1094</v>
       </c>
@@ -5302,6 +5316,9 @@
       <c r="E78">
         <v>2013</v>
       </c>
+      <c r="F78" t="s">
+        <v>26</v>
+      </c>
       <c r="H78">
         <v>48.856699999999996</v>
       </c>
@@ -5330,7 +5347,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22">
       <c r="A79">
         <v>1101</v>
       </c>
@@ -5346,6 +5363,9 @@
       <c r="E79">
         <v>2015</v>
       </c>
+      <c r="F79" t="s">
+        <v>396</v>
+      </c>
       <c r="H79">
         <v>-37.813609999999997</v>
       </c>
@@ -5377,7 +5397,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22">
       <c r="A80">
         <v>1105</v>
       </c>
@@ -5393,6 +5413,9 @@
       <c r="E80">
         <v>2014</v>
       </c>
+      <c r="F80" t="s">
+        <v>26</v>
+      </c>
       <c r="H80">
         <v>41.836944000000003</v>
       </c>
@@ -5421,7 +5444,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25">
       <c r="A81">
         <v>1107</v>
       </c>
@@ -5471,7 +5494,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25">
       <c r="A82">
         <v>1114</v>
       </c>
@@ -5518,7 +5541,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25">
       <c r="A83">
         <v>1120</v>
       </c>
@@ -5565,7 +5588,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25">
       <c r="A84">
         <v>1123</v>
       </c>
@@ -5609,7 +5632,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25">
       <c r="A85">
         <v>1126</v>
       </c>
@@ -5638,7 +5661,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25">
       <c r="A86">
         <v>1127</v>
       </c>
@@ -5673,7 +5696,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25">
       <c r="A87">
         <v>1134</v>
       </c>
@@ -5702,7 +5725,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25">
       <c r="A88">
         <v>1136</v>
       </c>
@@ -5731,7 +5754,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25">
       <c r="A89">
         <v>1137</v>
       </c>
@@ -5757,7 +5780,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25">
       <c r="A90">
         <v>1156</v>
       </c>
@@ -5807,7 +5830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25">
       <c r="A91">
         <v>1167</v>
       </c>
@@ -5854,7 +5877,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25">
       <c r="A92">
         <v>1198</v>
       </c>
@@ -5901,7 +5924,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25">
       <c r="A93">
         <v>1201</v>
       </c>
@@ -5951,7 +5974,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25">
       <c r="A94">
         <v>1223</v>
       </c>
@@ -5995,7 +6018,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25">
       <c r="A95">
         <v>1255</v>
       </c>
@@ -6042,7 +6065,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25">
       <c r="A96">
         <v>1262</v>
       </c>
@@ -6086,7 +6109,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="97" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22 16384:16384">
       <c r="A97">
         <v>1265</v>
       </c>
@@ -6133,7 +6156,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22 16384:16384">
       <c r="A98">
         <v>1267</v>
       </c>
@@ -6162,7 +6185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22 16384:16384">
       <c r="A99">
         <v>1269</v>
       </c>
@@ -6206,7 +6229,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22 16384:16384">
       <c r="A100">
         <v>1273</v>
       </c>
@@ -6235,7 +6258,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="101" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22 16384:16384">
       <c r="A101">
         <v>1274</v>
       </c>
@@ -6279,7 +6302,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22 16384:16384">
       <c r="A102">
         <v>1285</v>
       </c>
@@ -6326,7 +6349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22 16384:16384">
       <c r="A103">
         <v>1286</v>
       </c>
@@ -6370,7 +6393,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="104" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22 16384:16384">
       <c r="A104">
         <v>1287</v>
       </c>
@@ -6396,7 +6419,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="105" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22 16384:16384">
       <c r="A105">
         <v>1288</v>
       </c>
@@ -6425,7 +6448,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="106" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22 16384:16384">
       <c r="A106">
         <v>1289</v>
       </c>
@@ -6472,7 +6495,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22 16384:16384">
       <c r="A107">
         <v>1290</v>
       </c>
@@ -6519,7 +6542,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="108" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22 16384:16384">
       <c r="A108">
         <v>1291</v>
       </c>
@@ -6560,7 +6583,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="109" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22 16384:16384">
       <c r="A109">
         <v>1292</v>
       </c>
@@ -6601,7 +6624,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="110" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22 16384:16384">
       <c r="A110">
         <v>1293</v>
       </c>
@@ -6630,7 +6653,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="111" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22 16384:16384">
       <c r="A111">
         <v>1294</v>
       </c>
@@ -6662,7 +6685,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="112" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22 16384:16384">
       <c r="A112">
         <v>1295</v>
       </c>
@@ -6709,7 +6732,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17">
       <c r="A113">
         <v>1296</v>
       </c>
@@ -6756,7 +6779,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17">
       <c r="A114">
         <v>1297</v>
       </c>
@@ -6803,7 +6826,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17">
       <c r="A115">
         <v>1298</v>
       </c>
@@ -6850,7 +6873,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17">
       <c r="A116">
         <v>1299</v>
       </c>
@@ -6897,7 +6920,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17">
       <c r="A117">
         <v>1300</v>
       </c>
@@ -6944,7 +6967,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17">
       <c r="A118">
         <v>1301</v>
       </c>
@@ -6991,7 +7014,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17">
       <c r="A119">
         <v>1302</v>
       </c>
@@ -7038,7 +7061,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17">
       <c r="A120">
         <v>1303</v>
       </c>

</xml_diff>

<commit_message>
aggregated some additional datasets
</commit_message>
<xml_diff>
--- a/data/MSdata.xlsx
+++ b/data/MSdata.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PhD - 10th Year\GreenInfrastructureMeta\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="660" windowWidth="28275" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="471">
   <si>
     <t>id</t>
   </si>
@@ -1432,8 +1437,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1524,7 +1529,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1556,9 +1561,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1590,6 +1596,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1765,19 +1772,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1854,7 +1861,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>39</v>
       </c>
@@ -1889,7 +1896,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>69</v>
       </c>
@@ -1942,7 +1949,7 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>95</v>
       </c>
@@ -1986,7 +1993,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>
@@ -2033,7 +2040,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>150</v>
       </c>
@@ -2089,7 +2096,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>154</v>
       </c>
@@ -2136,7 +2143,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>161</v>
       </c>
@@ -2186,7 +2193,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>189</v>
       </c>
@@ -2236,7 +2243,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>247</v>
       </c>
@@ -2280,7 +2287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>251</v>
       </c>
@@ -2327,7 +2334,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>253</v>
       </c>
@@ -2377,7 +2384,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>310</v>
       </c>
@@ -2424,7 +2431,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>315</v>
       </c>
@@ -2456,7 +2463,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>319</v>
       </c>
@@ -2509,7 +2516,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>328</v>
       </c>
@@ -2556,7 +2563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>335</v>
       </c>
@@ -2603,7 +2610,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>356</v>
       </c>
@@ -2653,7 +2660,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>364</v>
       </c>
@@ -2700,7 +2707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>397</v>
       </c>
@@ -2732,7 +2739,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>400</v>
       </c>
@@ -2782,7 +2789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>408</v>
       </c>
@@ -2814,7 +2821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>415</v>
       </c>
@@ -2864,7 +2871,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>429</v>
       </c>
@@ -2911,7 +2918,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>431</v>
       </c>
@@ -2943,7 +2950,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>434</v>
       </c>
@@ -2990,7 +2997,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>454</v>
       </c>
@@ -3037,7 +3044,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>463</v>
       </c>
@@ -3084,7 +3091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>464</v>
       </c>
@@ -3131,7 +3138,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>465</v>
       </c>
@@ -3157,7 +3164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>466</v>
       </c>
@@ -3210,7 +3217,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>491</v>
       </c>
@@ -3254,7 +3261,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>499</v>
       </c>
@@ -3301,7 +3308,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>511</v>
       </c>
@@ -3333,7 +3340,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>514</v>
       </c>
@@ -3386,7 +3393,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>536</v>
       </c>
@@ -3442,7 +3449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>546</v>
       </c>
@@ -3486,7 +3493,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>563</v>
       </c>
@@ -3533,7 +3540,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>593</v>
       </c>
@@ -3574,7 +3581,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>621</v>
       </c>
@@ -3615,7 +3622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:22">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>640</v>
       </c>
@@ -3662,7 +3669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:22">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>641</v>
       </c>
@@ -3712,7 +3719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:22">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>659</v>
       </c>
@@ -3762,7 +3769,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:22">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>670</v>
       </c>
@@ -3791,7 +3798,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:22">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>679</v>
       </c>
@@ -3841,7 +3848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>697</v>
       </c>
@@ -3888,7 +3895,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:22">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>728</v>
       </c>
@@ -3917,7 +3924,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:22">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>760</v>
       </c>
@@ -3964,7 +3971,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>777</v>
       </c>
@@ -4011,7 +4018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>787</v>
       </c>
@@ -4058,7 +4065,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>800</v>
       </c>
@@ -4087,7 +4094,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>877</v>
       </c>
@@ -4128,7 +4135,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>879</v>
       </c>
@@ -4178,7 +4185,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>881</v>
       </c>
@@ -4228,7 +4235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>895</v>
       </c>
@@ -4278,7 +4285,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>899</v>
       </c>
@@ -4328,7 +4335,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>912</v>
       </c>
@@ -4369,7 +4376,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>926</v>
       </c>
@@ -4416,7 +4423,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>949</v>
       </c>
@@ -4454,7 +4461,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>976</v>
       </c>
@@ -4504,7 +4511,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1023</v>
       </c>
@@ -4548,7 +4555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1046</v>
       </c>
@@ -4589,7 +4596,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1047</v>
       </c>
@@ -4630,7 +4637,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1049</v>
       </c>
@@ -4680,7 +4687,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="65" spans="1:22">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1050</v>
       </c>
@@ -4733,7 +4740,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:22">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1051</v>
       </c>
@@ -4789,7 +4796,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:22">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1052</v>
       </c>
@@ -4836,7 +4843,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="68" spans="1:22">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1055</v>
       </c>
@@ -4886,7 +4893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:22">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1056</v>
       </c>
@@ -4933,7 +4940,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="70" spans="1:22">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1059</v>
       </c>
@@ -4965,7 +4972,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="71" spans="1:22">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1062</v>
       </c>
@@ -5015,7 +5022,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:22">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1063</v>
       </c>
@@ -5065,7 +5072,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="73" spans="1:22">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1067</v>
       </c>
@@ -5112,7 +5119,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="74" spans="1:22">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1069</v>
       </c>
@@ -5159,7 +5166,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="75" spans="1:22">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1070</v>
       </c>
@@ -5206,7 +5213,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="76" spans="1:22">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1076</v>
       </c>
@@ -5250,7 +5257,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:22">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1093</v>
       </c>
@@ -5300,7 +5307,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:22">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1094</v>
       </c>
@@ -5347,7 +5354,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:22">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1101</v>
       </c>
@@ -5397,7 +5404,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="80" spans="1:22">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1105</v>
       </c>
@@ -5444,7 +5451,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="81" spans="1:25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1107</v>
       </c>
@@ -5460,6 +5467,9 @@
       <c r="E81">
         <v>2011</v>
       </c>
+      <c r="F81" t="s">
+        <v>26</v>
+      </c>
       <c r="H81">
         <v>40.712777799999998</v>
       </c>
@@ -5494,7 +5504,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1114</v>
       </c>
@@ -5510,6 +5520,9 @@
       <c r="E82">
         <v>2014</v>
       </c>
+      <c r="F82" t="s">
+        <v>396</v>
+      </c>
       <c r="H82">
         <v>43.7</v>
       </c>
@@ -5541,7 +5554,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1120</v>
       </c>
@@ -5557,6 +5570,9 @@
       <c r="E83">
         <v>2014</v>
       </c>
+      <c r="F83" t="s">
+        <v>26</v>
+      </c>
       <c r="H83">
         <v>50.371389000000001</v>
       </c>
@@ -5588,7 +5604,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1123</v>
       </c>
@@ -5604,6 +5620,9 @@
       <c r="E84">
         <v>2015</v>
       </c>
+      <c r="F84" t="s">
+        <v>26</v>
+      </c>
       <c r="H84">
         <v>41.836944000000003</v>
       </c>
@@ -5632,7 +5651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1126</v>
       </c>
@@ -5648,6 +5667,9 @@
       <c r="E85">
         <v>2016</v>
       </c>
+      <c r="F85" t="s">
+        <v>26</v>
+      </c>
       <c r="L85" t="s">
         <v>105</v>
       </c>
@@ -5661,7 +5683,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="86" spans="1:25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1127</v>
       </c>
@@ -5677,6 +5699,9 @@
       <c r="E86">
         <v>2015</v>
       </c>
+      <c r="F86" t="s">
+        <v>26</v>
+      </c>
       <c r="H86">
         <v>50.802999999999997</v>
       </c>
@@ -5696,7 +5721,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="87" spans="1:25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1134</v>
       </c>
@@ -5725,7 +5750,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="88" spans="1:25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1136</v>
       </c>
@@ -5754,7 +5779,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="89" spans="1:25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1137</v>
       </c>
@@ -5780,7 +5805,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="90" spans="1:25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1156</v>
       </c>
@@ -5830,7 +5855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1167</v>
       </c>
@@ -5877,7 +5902,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="92" spans="1:25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1198</v>
       </c>
@@ -5924,7 +5949,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="93" spans="1:25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1201</v>
       </c>
@@ -5974,7 +5999,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="94" spans="1:25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1223</v>
       </c>
@@ -6018,7 +6043,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="95" spans="1:25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1255</v>
       </c>
@@ -6065,7 +6090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1262</v>
       </c>
@@ -6109,7 +6134,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="97" spans="1:22 16384:16384">
+    <row r="97" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1265</v>
       </c>
@@ -6156,7 +6181,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:22 16384:16384">
+    <row r="98" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1267</v>
       </c>
@@ -6185,7 +6210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:22 16384:16384">
+    <row r="99" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1269</v>
       </c>
@@ -6229,7 +6254,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:22 16384:16384">
+    <row r="100" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1273</v>
       </c>
@@ -6258,7 +6283,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="101" spans="1:22 16384:16384">
+    <row r="101" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1274</v>
       </c>
@@ -6302,7 +6327,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:22 16384:16384">
+    <row r="102" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1285</v>
       </c>
@@ -6349,7 +6374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:22 16384:16384">
+    <row r="103" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1286</v>
       </c>
@@ -6393,7 +6418,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="104" spans="1:22 16384:16384">
+    <row r="104" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1287</v>
       </c>
@@ -6419,7 +6444,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="105" spans="1:22 16384:16384">
+    <row r="105" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1288</v>
       </c>
@@ -6448,7 +6473,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="106" spans="1:22 16384:16384">
+    <row r="106" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1289</v>
       </c>
@@ -6495,7 +6520,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:22 16384:16384">
+    <row r="107" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1290</v>
       </c>
@@ -6542,7 +6567,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="108" spans="1:22 16384:16384">
+    <row r="108" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1291</v>
       </c>
@@ -6583,7 +6608,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="109" spans="1:22 16384:16384">
+    <row r="109" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1292</v>
       </c>
@@ -6624,7 +6649,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="110" spans="1:22 16384:16384">
+    <row r="110" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1293</v>
       </c>
@@ -6653,7 +6678,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="111" spans="1:22 16384:16384">
+    <row r="111" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1294</v>
       </c>
@@ -6685,7 +6710,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="112" spans="1:22 16384:16384">
+    <row r="112" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1295</v>
       </c>
@@ -6732,7 +6757,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="113" spans="1:17">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1296</v>
       </c>
@@ -6779,7 +6804,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="114" spans="1:17">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1297</v>
       </c>
@@ -6826,7 +6851,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1298</v>
       </c>
@@ -6873,7 +6898,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1299</v>
       </c>
@@ -6920,7 +6945,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1300</v>
       </c>
@@ -6967,7 +6992,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1301</v>
       </c>
@@ -7014,7 +7039,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1302</v>
       </c>
@@ -7061,7 +7086,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="120" spans="1:17">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1303</v>
       </c>

</xml_diff>

<commit_message>
finished collecting data online and begun generating a master dataset
</commit_message>
<xml_diff>
--- a/data/MSdata.xlsx
+++ b/data/MSdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="472">
   <si>
     <t>id</t>
   </si>
@@ -1432,6 +1432,9 @@
   </si>
   <si>
     <t>Inverness</t>
+  </si>
+  <si>
+    <t>stat.output</t>
   </si>
 </sst>
 </file>
@@ -1775,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O86" sqref="O86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4989,7 +4992,7 @@
         <v>2011</v>
       </c>
       <c r="F71" t="s">
-        <v>396</v>
+        <v>26</v>
       </c>
       <c r="H71">
         <v>52.483055999999998</v>
@@ -5737,6 +5740,9 @@
       <c r="E87">
         <v>2015</v>
       </c>
+      <c r="F87" t="s">
+        <v>471</v>
+      </c>
       <c r="L87" t="s">
         <v>27</v>
       </c>
@@ -5766,6 +5772,9 @@
       <c r="E88">
         <v>2014</v>
       </c>
+      <c r="F88" t="s">
+        <v>471</v>
+      </c>
       <c r="L88" t="s">
         <v>141</v>
       </c>
@@ -5795,6 +5804,9 @@
       <c r="E89">
         <v>2011</v>
       </c>
+      <c r="F89" t="s">
+        <v>471</v>
+      </c>
       <c r="L89" t="s">
         <v>355</v>
       </c>
@@ -5821,6 +5833,9 @@
       <c r="E90">
         <v>2014</v>
       </c>
+      <c r="F90" t="s">
+        <v>26</v>
+      </c>
       <c r="H90">
         <v>57.7</v>
       </c>
@@ -5871,6 +5886,9 @@
       <c r="E91">
         <v>2016</v>
       </c>
+      <c r="F91" t="s">
+        <v>26</v>
+      </c>
       <c r="H91">
         <v>52.516666999999998</v>
       </c>
@@ -5918,6 +5936,9 @@
       <c r="E92">
         <v>2017</v>
       </c>
+      <c r="F92" t="s">
+        <v>26</v>
+      </c>
       <c r="H92">
         <v>45.5</v>
       </c>
@@ -5965,6 +5986,9 @@
       <c r="E93">
         <v>2016</v>
       </c>
+      <c r="F93" t="s">
+        <v>400</v>
+      </c>
       <c r="H93">
         <v>33.450000000000003</v>
       </c>
@@ -6015,6 +6039,9 @@
       <c r="E94">
         <v>2018</v>
       </c>
+      <c r="F94" t="s">
+        <v>26</v>
+      </c>
       <c r="H94">
         <v>42.101388999999998</v>
       </c>
@@ -6059,6 +6086,9 @@
       <c r="E95">
         <v>2018</v>
       </c>
+      <c r="F95" t="s">
+        <v>26</v>
+      </c>
       <c r="H95">
         <v>48.179349999999999</v>
       </c>
@@ -6106,6 +6136,9 @@
       <c r="E96">
         <v>2018</v>
       </c>
+      <c r="F96" t="s">
+        <v>400</v>
+      </c>
       <c r="H96">
         <v>38.627222000000003</v>
       </c>
@@ -6150,6 +6183,9 @@
       <c r="E97">
         <v>2017</v>
       </c>
+      <c r="F97" t="s">
+        <v>26</v>
+      </c>
       <c r="H97">
         <v>46.816667000000002</v>
       </c>
@@ -6197,6 +6233,9 @@
       <c r="E98">
         <v>2017</v>
       </c>
+      <c r="F98" t="s">
+        <v>400</v>
+      </c>
       <c r="L98" t="s">
         <v>37</v>
       </c>
@@ -6226,6 +6265,9 @@
       <c r="E99">
         <v>2017</v>
       </c>
+      <c r="F99" t="s">
+        <v>26</v>
+      </c>
       <c r="H99">
         <v>41.665556000000002</v>
       </c>
@@ -6270,6 +6312,9 @@
       <c r="E100">
         <v>2017</v>
       </c>
+      <c r="F100" t="s">
+        <v>26</v>
+      </c>
       <c r="L100" t="s">
         <v>130</v>
       </c>
@@ -6299,6 +6344,9 @@
       <c r="E101">
         <v>2017</v>
       </c>
+      <c r="F101" t="s">
+        <v>26</v>
+      </c>
       <c r="H101">
         <v>-33.865000000000002</v>
       </c>
@@ -6343,6 +6391,9 @@
       <c r="E102">
         <v>2010</v>
       </c>
+      <c r="F102" t="s">
+        <v>396</v>
+      </c>
       <c r="H102">
         <v>44.647778000000002</v>
       </c>
@@ -6390,6 +6441,9 @@
       <c r="E103">
         <v>2013</v>
       </c>
+      <c r="F103" t="s">
+        <v>26</v>
+      </c>
       <c r="H103">
         <v>53.010899999999999</v>
       </c>
@@ -6434,6 +6488,9 @@
       <c r="E104">
         <v>2006</v>
       </c>
+      <c r="F104" t="s">
+        <v>26</v>
+      </c>
       <c r="L104" t="s">
         <v>176</v>
       </c>
@@ -6583,6 +6640,9 @@
       <c r="E108">
         <v>2012</v>
       </c>
+      <c r="F108" t="s">
+        <v>400</v>
+      </c>
       <c r="H108">
         <v>41.836944000000003</v>
       </c>
@@ -6623,6 +6683,9 @@
       </c>
       <c r="E109">
         <v>2011</v>
+      </c>
+      <c r="F109" t="s">
+        <v>26</v>
       </c>
       <c r="H109">
         <v>41.836944000000003</v>

</xml_diff>

<commit_message>
added two datasets that were emailed to me
</commit_message>
<xml_diff>
--- a/data/MSdata.xlsx
+++ b/data/MSdata.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1778,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O86" sqref="O86"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4616,7 +4616,7 @@
         <v>2011</v>
       </c>
       <c r="F63" t="s">
-        <v>396</v>
+        <v>26</v>
       </c>
       <c r="H63">
         <v>39.823430000000002</v>

</xml_diff>

<commit_message>
completed generating master dataset of all GI and raw data
</commit_message>
<xml_diff>
--- a/data/MSdata.xlsx
+++ b/data/MSdata.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1778,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,7 +2483,7 @@
         <v>2017</v>
       </c>
       <c r="F15" t="s">
-        <v>396</v>
+        <v>26</v>
       </c>
       <c r="H15">
         <v>-37.813609999999997</v>
@@ -6978,7 +6978,7 @@
         <v>2014</v>
       </c>
       <c r="F116" t="s">
-        <v>396</v>
+        <v>26</v>
       </c>
       <c r="H116">
         <v>47.366667</v>

</xml_diff>

<commit_message>
updated analyses as discussed: dropped relative abundance, added partridge paper, cleaned up nat vs GI comparison
</commit_message>
<xml_diff>
--- a/data/MSdata.xlsx
+++ b/data/MSdata.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PhD - 10th Year\GreenInfrastructureMeta\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="660" windowWidth="28275" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="477">
   <si>
     <t>id</t>
   </si>
@@ -1430,13 +1435,28 @@
   </si>
   <si>
     <t>stat.output</t>
+  </si>
+  <si>
+    <t>Urban green roofs provide habitat for migrating and breeding birds and their arthropod prey</t>
+  </si>
+  <si>
+    <t>Partridge, D., &amp; Clark, J.A.</t>
+  </si>
+  <si>
+    <t>bird composition</t>
+  </si>
+  <si>
+    <t>Stormwater wetlands for the enhancement of environmental ecosystem services: case studies for two retrofit wetlands in Brisbane, Australia</t>
+  </si>
+  <si>
+    <t>Journal of Cleaner Production</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1527,7 +1547,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1559,9 +1579,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1593,6 +1614,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1768,19 +1790,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD120"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFD123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M124" sqref="M124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1857,7 +1879,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>39</v>
       </c>
@@ -1892,7 +1914,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>69</v>
       </c>
@@ -1945,7 +1967,7 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>95</v>
       </c>
@@ -1989,7 +2011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>
@@ -2036,7 +2058,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>150</v>
       </c>
@@ -2092,7 +2114,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>154</v>
       </c>
@@ -2139,7 +2161,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>161</v>
       </c>
@@ -2189,7 +2211,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>189</v>
       </c>
@@ -2239,7 +2261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>247</v>
       </c>
@@ -2283,7 +2305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>251</v>
       </c>
@@ -2330,7 +2352,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>253</v>
       </c>
@@ -2380,7 +2402,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>310</v>
       </c>
@@ -2427,7 +2449,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>315</v>
       </c>
@@ -2459,7 +2481,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>319</v>
       </c>
@@ -2512,7 +2534,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>328</v>
       </c>
@@ -2559,7 +2581,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>335</v>
       </c>
@@ -2606,7 +2628,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>356</v>
       </c>
@@ -2656,7 +2678,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>364</v>
       </c>
@@ -2703,7 +2725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>397</v>
       </c>
@@ -2735,7 +2757,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>400</v>
       </c>
@@ -2785,7 +2807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>408</v>
       </c>
@@ -2817,7 +2839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>415</v>
       </c>
@@ -2867,7 +2889,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>429</v>
       </c>
@@ -2914,7 +2936,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>431</v>
       </c>
@@ -2946,7 +2968,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>434</v>
       </c>
@@ -2993,7 +3015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>454</v>
       </c>
@@ -3040,7 +3062,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>463</v>
       </c>
@@ -3087,7 +3109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>464</v>
       </c>
@@ -3134,7 +3156,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>465</v>
       </c>
@@ -3160,7 +3182,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>466</v>
       </c>
@@ -3213,7 +3235,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>491</v>
       </c>
@@ -3257,7 +3279,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>499</v>
       </c>
@@ -3304,7 +3326,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>511</v>
       </c>
@@ -3336,7 +3358,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>514</v>
       </c>
@@ -3389,7 +3411,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>536</v>
       </c>
@@ -3445,7 +3467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>546</v>
       </c>
@@ -3489,7 +3511,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>563</v>
       </c>
@@ -3536,7 +3558,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>593</v>
       </c>
@@ -3577,7 +3599,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>621</v>
       </c>
@@ -3618,7 +3640,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:22">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>640</v>
       </c>
@@ -3665,7 +3687,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:22">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>641</v>
       </c>
@@ -3715,7 +3737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:22">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>659</v>
       </c>
@@ -3765,7 +3787,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:22">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>670</v>
       </c>
@@ -3794,7 +3816,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:22">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>679</v>
       </c>
@@ -3844,7 +3866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>697</v>
       </c>
@@ -3891,7 +3913,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:22">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>728</v>
       </c>
@@ -3920,7 +3942,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:22">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>760</v>
       </c>
@@ -3967,7 +3989,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>777</v>
       </c>
@@ -4014,7 +4036,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>787</v>
       </c>
@@ -4061,7 +4083,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>800</v>
       </c>
@@ -4090,7 +4112,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>877</v>
       </c>
@@ -4131,7 +4153,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>879</v>
       </c>
@@ -4181,7 +4203,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>881</v>
       </c>
@@ -4231,7 +4253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>895</v>
       </c>
@@ -4281,7 +4303,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>899</v>
       </c>
@@ -4331,7 +4353,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>912</v>
       </c>
@@ -4372,21 +4394,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>926</v>
       </c>
       <c r="B58" t="s">
-        <v>404</v>
+        <v>475</v>
       </c>
       <c r="C58" t="s">
         <v>254</v>
       </c>
       <c r="D58" t="s">
-        <v>255</v>
+        <v>476</v>
       </c>
       <c r="E58">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="F58" t="s">
         <v>26</v>
@@ -4413,13 +4435,13 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="O58" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="Q58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>949</v>
       </c>
@@ -4457,7 +4479,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>976</v>
       </c>
@@ -4507,7 +4529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1023</v>
       </c>
@@ -4551,7 +4573,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1046</v>
       </c>
@@ -4592,7 +4614,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1047</v>
       </c>
@@ -4633,7 +4655,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1049</v>
       </c>
@@ -4683,7 +4705,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="65" spans="1:22">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1050</v>
       </c>
@@ -4736,7 +4758,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:22">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1051</v>
       </c>
@@ -4792,7 +4814,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:22">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1052</v>
       </c>
@@ -4839,7 +4861,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="68" spans="1:22">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1055</v>
       </c>
@@ -4889,7 +4911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:22">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1056</v>
       </c>
@@ -4936,7 +4958,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="70" spans="1:22">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1059</v>
       </c>
@@ -4968,7 +4990,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="71" spans="1:22">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1062</v>
       </c>
@@ -5018,7 +5040,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:22">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1063</v>
       </c>
@@ -5068,7 +5090,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="73" spans="1:22">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1067</v>
       </c>
@@ -5115,7 +5137,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="74" spans="1:22">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1069</v>
       </c>
@@ -5162,7 +5184,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="75" spans="1:22">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1070</v>
       </c>
@@ -5209,7 +5231,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="76" spans="1:22">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1076</v>
       </c>
@@ -5253,7 +5275,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:22">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1093</v>
       </c>
@@ -5303,7 +5325,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:22">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1094</v>
       </c>
@@ -5350,7 +5372,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:22">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1101</v>
       </c>
@@ -5400,7 +5422,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="80" spans="1:22">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1105</v>
       </c>
@@ -5447,7 +5469,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="81" spans="1:25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1107</v>
       </c>
@@ -5500,7 +5522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1114</v>
       </c>
@@ -5550,7 +5572,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1120</v>
       </c>
@@ -5600,7 +5622,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1123</v>
       </c>
@@ -5647,7 +5669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1126</v>
       </c>
@@ -5679,7 +5701,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="86" spans="1:25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1127</v>
       </c>
@@ -5717,7 +5739,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="87" spans="1:25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1134</v>
       </c>
@@ -5749,7 +5771,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="88" spans="1:25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1136</v>
       </c>
@@ -5781,7 +5803,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="89" spans="1:25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1137</v>
       </c>
@@ -5810,7 +5832,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="90" spans="1:25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1156</v>
       </c>
@@ -5863,7 +5885,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1167</v>
       </c>
@@ -5913,7 +5935,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="92" spans="1:25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1198</v>
       </c>
@@ -5963,7 +5985,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="93" spans="1:25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1201</v>
       </c>
@@ -6016,7 +6038,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="94" spans="1:25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1223</v>
       </c>
@@ -6063,7 +6085,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="95" spans="1:25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1255</v>
       </c>
@@ -6113,7 +6135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1262</v>
       </c>
@@ -6160,7 +6182,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="97" spans="1:22 16384:16384">
+    <row r="97" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1265</v>
       </c>
@@ -6210,7 +6232,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:22 16384:16384">
+    <row r="98" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1267</v>
       </c>
@@ -6242,7 +6264,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:22 16384:16384">
+    <row r="99" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1269</v>
       </c>
@@ -6289,7 +6311,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:22 16384:16384">
+    <row r="100" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1273</v>
       </c>
@@ -6321,7 +6343,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="101" spans="1:22 16384:16384">
+    <row r="101" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1274</v>
       </c>
@@ -6368,7 +6390,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:22 16384:16384">
+    <row r="102" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1285</v>
       </c>
@@ -6418,7 +6440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:22 16384:16384">
+    <row r="103" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1286</v>
       </c>
@@ -6465,7 +6487,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="104" spans="1:22 16384:16384">
+    <row r="104" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1287</v>
       </c>
@@ -6494,7 +6516,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="105" spans="1:22 16384:16384">
+    <row r="105" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1288</v>
       </c>
@@ -6523,7 +6545,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="106" spans="1:22 16384:16384">
+    <row r="106" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1289</v>
       </c>
@@ -6570,7 +6592,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:22 16384:16384">
+    <row r="107" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1290</v>
       </c>
@@ -6617,7 +6639,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="108" spans="1:22 16384:16384">
+    <row r="108" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1291</v>
       </c>
@@ -6661,7 +6683,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="109" spans="1:22 16384:16384">
+    <row r="109" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1292</v>
       </c>
@@ -6705,7 +6727,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="110" spans="1:22 16384:16384">
+    <row r="110" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1293</v>
       </c>
@@ -6734,7 +6756,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="111" spans="1:22 16384:16384">
+    <row r="111" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1294</v>
       </c>
@@ -6766,7 +6788,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="112" spans="1:22 16384:16384">
+    <row r="112" spans="1:22 16384:16384" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1295</v>
       </c>
@@ -6813,7 +6835,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="113" spans="1:17">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1296</v>
       </c>
@@ -6860,7 +6882,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="114" spans="1:17">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1297</v>
       </c>
@@ -6907,7 +6929,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1298</v>
       </c>
@@ -6954,7 +6976,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1299</v>
       </c>
@@ -7001,7 +7023,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1300</v>
       </c>
@@ -7048,7 +7070,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1301</v>
       </c>
@@ -7095,7 +7117,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1302</v>
       </c>
@@ -7142,7 +7164,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="120" spans="1:17">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1303</v>
       </c>
@@ -7186,6 +7208,105 @@
         <v>33</v>
       </c>
       <c r="Q120" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>1305</v>
+      </c>
+      <c r="B122" t="s">
+        <v>472</v>
+      </c>
+      <c r="C122" t="s">
+        <v>473</v>
+      </c>
+      <c r="D122" t="s">
+        <v>301</v>
+      </c>
+      <c r="E122">
+        <v>2018</v>
+      </c>
+      <c r="F122" t="s">
+        <v>26</v>
+      </c>
+      <c r="H122">
+        <v>40.712777799999998</v>
+      </c>
+      <c r="I122">
+        <v>-74.005832999999996</v>
+      </c>
+      <c r="J122">
+        <v>10</v>
+      </c>
+      <c r="K122" t="s">
+        <v>192</v>
+      </c>
+      <c r="L122" t="s">
+        <v>37</v>
+      </c>
+      <c r="M122">
+        <v>8.6219999999999999</v>
+      </c>
+      <c r="N122">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="O122" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>1306</v>
+      </c>
+      <c r="B123" t="s">
+        <v>404</v>
+      </c>
+      <c r="C123" t="s">
+        <v>254</v>
+      </c>
+      <c r="D123" t="s">
+        <v>255</v>
+      </c>
+      <c r="E123">
+        <v>2014</v>
+      </c>
+      <c r="F123" t="s">
+        <v>26</v>
+      </c>
+      <c r="H123">
+        <v>-27.466667000000001</v>
+      </c>
+      <c r="I123">
+        <v>153.033333</v>
+      </c>
+      <c r="J123">
+        <v>8</v>
+      </c>
+      <c r="K123" t="s">
+        <v>409</v>
+      </c>
+      <c r="L123" t="s">
+        <v>105</v>
+      </c>
+      <c r="M123">
+        <v>2.4082330000000001</v>
+      </c>
+      <c r="N123">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="O123" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q123" t="s">
         <v>267</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added two additional datasets
</commit_message>
<xml_diff>
--- a/data/MSdata.xlsx
+++ b/data/MSdata.xlsx
@@ -1793,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M124" sqref="M124"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,7 +2322,7 @@
         <v>2016</v>
       </c>
       <c r="F11" t="s">
-        <v>396</v>
+        <v>26</v>
       </c>
       <c r="H11">
         <v>43.7</v>
@@ -6899,7 +6899,7 @@
         <v>2012</v>
       </c>
       <c r="F114" t="s">
-        <v>396</v>
+        <v>26</v>
       </c>
       <c r="H114">
         <v>51.507221999999999</v>

</xml_diff>

<commit_message>
added two additional datasets and added some analyses for the technical report
</commit_message>
<xml_diff>
--- a/data/MSdata.xlsx
+++ b/data/MSdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="483">
   <si>
     <t>id</t>
   </si>
@@ -1445,6 +1445,24 @@
   </si>
   <si>
     <t>Journal of Cleaner Production</t>
+  </si>
+  <si>
+    <t>Unique Bee Communities within Vacant Lots and Urban Farms Result from Variation in Surrounding Urbanization Intensity</t>
+  </si>
+  <si>
+    <t>Sivakoff et al. 2018</t>
+  </si>
+  <si>
+    <t>Sustainability</t>
+  </si>
+  <si>
+    <t>Plant and microbial biodiversity in urban forests and public gardens: Insights for cities’ sustainable development</t>
+  </si>
+  <si>
+    <t>Lurdes Barrico, Helena Castro, António Pereira Coutinho, Maria Teresa Gonçalves, Helena Freitas, &amp; Paula Castro</t>
+  </si>
+  <si>
+    <t>Coimbra</t>
   </si>
 </sst>
 </file>
@@ -1784,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD123"/>
+  <dimension ref="A1:XFD125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C100" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M119" sqref="M119"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P128" sqref="P128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7303,6 +7321,100 @@
         <v>267</v>
       </c>
     </row>
+    <row r="124" spans="1:17">
+      <c r="A124">
+        <v>1307</v>
+      </c>
+      <c r="B124" t="s">
+        <v>477</v>
+      </c>
+      <c r="C124" t="s">
+        <v>478</v>
+      </c>
+      <c r="D124" t="s">
+        <v>479</v>
+      </c>
+      <c r="E124">
+        <v>2018</v>
+      </c>
+      <c r="F124" t="s">
+        <v>26</v>
+      </c>
+      <c r="H124">
+        <v>41.482222</v>
+      </c>
+      <c r="I124">
+        <v>-81.669721999999993</v>
+      </c>
+      <c r="J124">
+        <v>199</v>
+      </c>
+      <c r="K124" t="s">
+        <v>180</v>
+      </c>
+      <c r="L124" t="s">
+        <v>37</v>
+      </c>
+      <c r="M124">
+        <v>0.396698</v>
+      </c>
+      <c r="N124">
+        <v>1.8619999999999999E-3</v>
+      </c>
+      <c r="O124" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
+      <c r="A125">
+        <v>1308</v>
+      </c>
+      <c r="B125" t="s">
+        <v>480</v>
+      </c>
+      <c r="C125" t="s">
+        <v>481</v>
+      </c>
+      <c r="D125" t="s">
+        <v>57</v>
+      </c>
+      <c r="E125">
+        <v>2018</v>
+      </c>
+      <c r="F125" t="s">
+        <v>26</v>
+      </c>
+      <c r="H125">
+        <v>40.211111000000002</v>
+      </c>
+      <c r="I125">
+        <v>-8.4291669999999996</v>
+      </c>
+      <c r="J125">
+        <v>9</v>
+      </c>
+      <c r="K125" t="s">
+        <v>482</v>
+      </c>
+      <c r="L125" t="s">
+        <v>70</v>
+      </c>
+      <c r="M125">
+        <v>0.143396</v>
+      </c>
+      <c r="N125">
+        <v>3.19E-4</v>
+      </c>
+      <c r="O125" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>379</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>